<commit_message>
Sync local repository with Github
</commit_message>
<xml_diff>
--- a/data/Controls.xlsx
+++ b/data/Controls.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\HUCA LABORATORIO\1. Proyectos Tesis Doctoral\Mental disorders\STRs\Draft\Molecular Psychiatric\Mental-disorders-STRs\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\HUCA LABORATORIO\1. Proyectos Tesis Doctoral\04. Mental disorders\STRs\Draft\Molecular Psychiatric\Mental-disorders-STRs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FEE58E-5F92-4339-9D16-7D4B089E80EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975FE46D-311B-4A2F-8C64-70319D727667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3675,10 +3675,10 @@
   <dimension ref="A1:N1072"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B1026" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B545" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D564" sqref="D564"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -26995,10 +26995,10 @@
         <v>2</v>
       </c>
       <c r="C563" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D563" s="6">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="E563" s="6"/>
       <c r="F563" s="6">

</xml_diff>